<commit_message>
fix binary tree problem
</commit_message>
<xml_diff>
--- a/output_frameBTC.xlsx
+++ b/output_frameBTC.xlsx
@@ -407,7 +407,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="n">
-        <v>3852.32754613</v>
+        <v>2686.97731952</v>
       </c>
       <c r="C2" t="n">
         <v>0</v>
@@ -418,10 +418,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="n">
-        <v>3858.05495992</v>
+        <v>2709.1707084</v>
       </c>
       <c r="C3" t="n">
-        <v>0.001486741125051205</v>
+        <v>0.008259611541479028</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -429,10 +429,10 @@
         <v>4</v>
       </c>
       <c r="B4" t="n">
-        <v>4295.875037999999</v>
+        <v>2968.538408</v>
       </c>
       <c r="C4" t="n">
-        <v>0.1151375334933762</v>
+        <v>0.1047872962806764</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -440,10 +440,10 @@
         <v>5</v>
       </c>
       <c r="B5" t="n">
-        <v>4302.01</v>
+        <v>3057.67</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1167300673385743</v>
+        <v>0.1379589912378645</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -451,10 +451,10 @@
         <v>6</v>
       </c>
       <c r="B6" t="n">
-        <v>4311.72</v>
+        <v>3058.56</v>
       </c>
       <c r="C6" t="n">
-        <v>0.1192506214409259</v>
+        <v>0.1382902184475376</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -462,10 +462,10 @@
         <v>7</v>
       </c>
       <c r="B7" t="n">
-        <v>4313.4</v>
+        <v>3070.7</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1196867214297981</v>
+        <v>0.1428083064536427</v>
       </c>
     </row>
   </sheetData>

</xml_diff>